<commit_message>
Add Print Receipt Class
</commit_message>
<xml_diff>
--- a/Receipts/recepits.xlsx
+++ b/Receipts/recepits.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27374" windowHeight="11947"/>
+    <workbookView windowWidth="13687" windowHeight="11805"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,16 +40,16 @@
     <t>Acc.</t>
   </si>
   <si>
-    <t>Cumpulsory Deposite</t>
+    <t>Cumpulsory deposit</t>
   </si>
   <si>
     <t>Fine On CD</t>
   </si>
   <si>
-    <t>Loan Instalement</t>
+    <t>Loan Installment</t>
   </si>
   <si>
-    <t>Loan Interst</t>
+    <t>Loan Interest</t>
   </si>
   <si>
     <t>Fine On Loan</t>
@@ -61,7 +61,7 @@
     <t>Admission Fee</t>
   </si>
   <si>
-    <t>Welfare Deposite</t>
+    <t>Welfare deposit</t>
   </si>
   <si>
     <t>Misc. Deposit</t>
@@ -79,10 +79,10 @@
     <t>Share Money Balance</t>
   </si>
   <si>
-    <t>Cumpulsory Deposite Balance</t>
+    <t>Cumpulsory deposit Balance</t>
   </si>
   <si>
-    <t>Loan Instalement Balance</t>
+    <t>Loan Installment Balance</t>
   </si>
   <si>
     <t>Auth. Signatory</t>
@@ -144,33 +144,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -189,9 +191,62 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -206,62 +261,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -281,7 +281,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,79 +296,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,103 +470,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,17 +602,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -647,17 +665,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -673,15 +691,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -690,27 +699,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -731,131 +725,131 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -866,9 +860,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -928,34 +919,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -982,9 +952,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1309,313 +1276,315 @@
   </sheetPr>
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="27.66" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12.83" style="4" customWidth="1"/>
-    <col min="3" max="4" width="4.7" style="4" customWidth="1"/>
-    <col min="5" max="5" width="27.66" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.83" style="4" customWidth="1"/>
-    <col min="7" max="7" width="9.14" style="4"/>
-    <col min="8" max="8" width="11.69" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="9.14" style="4"/>
+    <col min="1" max="1" width="27.66" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83" style="1" customWidth="1"/>
+    <col min="3" max="4" width="4.7" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.66" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.14" style="1"/>
+    <col min="8" max="8" width="11.69" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.14" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="12" customHeight="1" spans="1:9">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7"/>
-      <c r="E1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="6"/>
-      <c r="H1" s="8" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="E1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="H1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="39">
+      <c r="I1" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="2" ht="12" customHeight="1" spans="1:6">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
-      <c r="E2" s="9" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10"/>
+      <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="10"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" ht="12" customHeight="1" spans="1:6">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="E3" s="12" t="s">
+      <c r="C3" s="13"/>
+      <c r="E3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" ht="12" customHeight="1" spans="1:6">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="E4" s="15" t="s">
+      <c r="C4" s="13"/>
+      <c r="E4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:6">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="17">
-        <v>0</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="E5" s="17" t="s">
+      <c r="B5" s="16">
+        <v>0</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="E5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="19">
-        <v>0</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="E6" s="19" t="s">
+      <c r="B6" s="18">
+        <v>0</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="E6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:6">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="19">
-        <v>0</v>
-      </c>
-      <c r="C7" s="18"/>
-      <c r="E7" s="19" t="s">
+      <c r="B7" s="18">
+        <v>0</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="E7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:6">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="19">
-        <v>0</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="E8" s="19" t="s">
+      <c r="B8" s="18">
+        <v>0</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="E8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:6">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="19">
-        <v>0</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="E9" s="19" t="s">
+      <c r="B9" s="18">
+        <v>0</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="E9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:6">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="19">
-        <v>0</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="E10" s="19" t="s">
+      <c r="B10" s="18">
+        <v>0</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="E10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:6">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="19">
-        <v>0</v>
-      </c>
-      <c r="C11" s="18"/>
-      <c r="E11" s="19" t="s">
+      <c r="B11" s="18">
+        <v>0</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="E11" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:6">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="19">
-        <v>0</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="E12" s="19" t="s">
+      <c r="B12" s="18">
+        <v>0</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="E12" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:6">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="20">
-        <v>0</v>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="E13" s="20" t="s">
+      <c r="B13" s="19">
+        <v>0</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="E13" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="14" customHeight="1" spans="1:6">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="22">
-        <v>0</v>
-      </c>
-      <c r="C14" s="23"/>
-      <c r="E14" s="21" t="s">
+      <c r="B14" s="21">
+        <f>SUM(B5:B13)</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="E14" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="21">
+        <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" customHeight="1" spans="1:6">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="24">
-        <v>0</v>
-      </c>
-      <c r="C15" s="25"/>
-      <c r="E15" s="17" t="s">
+      <c r="B15" s="16">
+        <v>0</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="E15" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="24">
+      <c r="F15" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="1:6">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="26">
-        <v>0</v>
-      </c>
-      <c r="C16" s="25"/>
-      <c r="E16" s="20" t="s">
+      <c r="B16" s="19">
+        <v>0</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="E16" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="1:6">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="28">
-        <v>0</v>
-      </c>
-      <c r="C17" s="23"/>
-      <c r="E17" s="29" t="s">
+      <c r="B17" s="22">
+        <v>0</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="E17" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="30">
+      <c r="F17" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="1:6">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="28">
-        <v>0</v>
-      </c>
-      <c r="C18" s="23"/>
-      <c r="E18" s="27" t="s">
+      <c r="B18" s="22">
+        <v>0</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="E18" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="28">
+      <c r="F18" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="1:6">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="32">
-        <v>0</v>
-      </c>
-      <c r="C19" s="23"/>
-      <c r="E19" s="31" t="s">
+      <c r="B19" s="24">
+        <v>0</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="E19" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="32">
+      <c r="F19" s="24">
         <v>0</v>
       </c>
     </row>
     <row r="20" ht="12" customHeight="1" spans="1:6">
-      <c r="A20" s="33"/>
-      <c r="B20" s="34" t="s">
+      <c r="A20" s="25"/>
+      <c r="B20" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="35"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="34" t="s">
+      <c r="C20" s="27"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="26" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1632,48 +1601,45 @@
       <c r="I22"/>
     </row>
     <row r="23" ht="12" customHeight="1" spans="1:9">
-      <c r="A23" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F23" s="6"/>
+      <c r="A23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="E23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="5"/>
       <c r="G23"/>
       <c r="H23"/>
       <c r="I23"/>
     </row>
     <row r="24" ht="12" customHeight="1" spans="1:9">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="9" t="s">
+      <c r="B24" s="9"/>
+      <c r="C24" s="10"/>
+      <c r="E24" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="10"/>
+      <c r="F24" s="9"/>
       <c r="G24"/>
       <c r="H24"/>
       <c r="I24"/>
     </row>
     <row r="25" ht="12" customHeight="1" spans="1:9">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="12" t="s">
+      <c r="C25" s="13"/>
+      <c r="E25" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="F25" s="12" t="s">
         <v>4</v>
       </c>
       <c r="G25"/>
@@ -1681,18 +1647,17 @@
       <c r="I25"/>
     </row>
     <row r="26" ht="12" customHeight="1" spans="1:9">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="15" t="s">
+      <c r="C26" s="13"/>
+      <c r="E26" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="F26" s="15" t="s">
         <v>6</v>
       </c>
       <c r="G26"/>
@@ -1700,18 +1665,17 @@
       <c r="I26"/>
     </row>
     <row r="27" customHeight="1" spans="1:9">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="17">
-        <v>0</v>
-      </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="17" t="s">
+      <c r="B27" s="16">
+        <v>0</v>
+      </c>
+      <c r="C27" s="17"/>
+      <c r="E27" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="17">
+      <c r="F27" s="16">
         <v>0</v>
       </c>
       <c r="G27"/>
@@ -1719,18 +1683,17 @@
       <c r="I27"/>
     </row>
     <row r="28" customHeight="1" spans="1:9">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="19">
-        <v>0</v>
-      </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="19" t="s">
+      <c r="B28" s="18">
+        <v>0</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="E28" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="19">
+      <c r="F28" s="18">
         <v>0</v>
       </c>
       <c r="G28"/>
@@ -1738,18 +1701,17 @@
       <c r="I28"/>
     </row>
     <row r="29" customHeight="1" spans="1:9">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="19">
-        <v>0</v>
-      </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="19" t="s">
+      <c r="B29" s="18">
+        <v>0</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="E29" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="19">
+      <c r="F29" s="18">
         <v>0</v>
       </c>
       <c r="G29"/>
@@ -1757,18 +1719,17 @@
       <c r="I29"/>
     </row>
     <row r="30" customHeight="1" spans="1:9">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="19">
-        <v>0</v>
-      </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="19" t="s">
+      <c r="B30" s="18">
+        <v>0</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="E30" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F30" s="19">
+      <c r="F30" s="18">
         <v>0</v>
       </c>
       <c r="G30"/>
@@ -1776,18 +1737,17 @@
       <c r="I30"/>
     </row>
     <row r="31" customHeight="1" spans="1:9">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="19">
-        <v>0</v>
-      </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="19" t="s">
+      <c r="B31" s="18">
+        <v>0</v>
+      </c>
+      <c r="C31" s="17"/>
+      <c r="E31" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="19">
+      <c r="F31" s="18">
         <v>0</v>
       </c>
       <c r="G31"/>
@@ -1795,18 +1755,17 @@
       <c r="I31"/>
     </row>
     <row r="32" customHeight="1" spans="1:9">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="19">
-        <v>0</v>
-      </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="19" t="s">
+      <c r="B32" s="18">
+        <v>0</v>
+      </c>
+      <c r="C32" s="17"/>
+      <c r="E32" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="19">
+      <c r="F32" s="18">
         <v>0</v>
       </c>
       <c r="G32"/>
@@ -1814,18 +1773,17 @@
       <c r="I32"/>
     </row>
     <row r="33" customHeight="1" spans="1:9">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="19">
-        <v>0</v>
-      </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="19" t="s">
+      <c r="B33" s="18">
+        <v>0</v>
+      </c>
+      <c r="C33" s="17"/>
+      <c r="E33" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F33" s="19">
+      <c r="F33" s="18">
         <v>0</v>
       </c>
       <c r="G33"/>
@@ -1833,18 +1791,17 @@
       <c r="I33"/>
     </row>
     <row r="34" customHeight="1" spans="1:9">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="19">
-        <v>0</v>
-      </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="19" t="s">
+      <c r="B34" s="18">
+        <v>0</v>
+      </c>
+      <c r="C34" s="17"/>
+      <c r="E34" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="19">
+      <c r="F34" s="18">
         <v>0</v>
       </c>
       <c r="G34"/>
@@ -1852,18 +1809,17 @@
       <c r="I34"/>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="20">
-        <v>0</v>
-      </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="20" t="s">
+      <c r="B35" s="19">
+        <v>0</v>
+      </c>
+      <c r="C35" s="17"/>
+      <c r="E35" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F35" s="20">
+      <c r="F35" s="19">
         <v>0</v>
       </c>
       <c r="G35"/>
@@ -1871,37 +1827,38 @@
       <c r="I35"/>
     </row>
     <row r="36" s="2" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A36" s="21" t="s">
+      <c r="A36" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="22">
-        <v>0</v>
-      </c>
-      <c r="C36" s="36"/>
+      <c r="B36" s="21">
+        <f>SUM(B27:B35)</f>
+        <v>0</v>
+      </c>
+      <c r="C36" s="28"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="21" t="s">
+      <c r="E36" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="22">
-        <v>0</v>
-      </c>
-      <c r="G36" s="37"/>
-      <c r="H36" s="37"/>
-      <c r="I36" s="37"/>
+      <c r="F36" s="21">
+        <f>SUM(F27:F35)</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
     </row>
     <row r="37" customHeight="1" spans="1:9">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="24">
-        <v>0</v>
-      </c>
-      <c r="C37" s="25"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="17" t="s">
+      <c r="B37" s="16">
+        <v>0</v>
+      </c>
+      <c r="C37" s="17"/>
+      <c r="E37" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="24">
+      <c r="F37" s="16">
         <v>0</v>
       </c>
       <c r="G37"/>
@@ -1909,18 +1866,17 @@
       <c r="I37"/>
     </row>
     <row r="38" customHeight="1" spans="1:9">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="26">
-        <v>0</v>
-      </c>
-      <c r="C38" s="25"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="20" t="s">
+      <c r="B38" s="19">
+        <v>0</v>
+      </c>
+      <c r="C38" s="17"/>
+      <c r="E38" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F38" s="26">
+      <c r="F38" s="19">
         <v>0</v>
       </c>
       <c r="G38"/>
@@ -1928,18 +1884,17 @@
       <c r="I38"/>
     </row>
     <row r="39" customHeight="1" spans="1:9">
-      <c r="A39" s="27" t="s">
+      <c r="A39" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="28">
-        <v>0</v>
-      </c>
-      <c r="C39" s="23"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="29" t="s">
+      <c r="B39" s="22">
+        <v>0</v>
+      </c>
+      <c r="C39" s="13"/>
+      <c r="E39" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="F39" s="30">
+      <c r="F39" s="23">
         <v>0</v>
       </c>
       <c r="G39"/>
@@ -1947,18 +1902,17 @@
       <c r="I39"/>
     </row>
     <row r="40" customHeight="1" spans="1:9">
-      <c r="A40" s="27" t="s">
+      <c r="A40" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="28">
-        <v>0</v>
-      </c>
-      <c r="C40" s="23"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="27" t="s">
+      <c r="B40" s="22">
+        <v>0</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="E40" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F40" s="28">
+      <c r="F40" s="22">
         <v>0</v>
       </c>
       <c r="G40"/>
@@ -1966,18 +1920,17 @@
       <c r="I40"/>
     </row>
     <row r="41" customHeight="1" spans="1:9">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="32">
-        <v>0</v>
-      </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="31" t="s">
+      <c r="B41" s="24">
+        <v>0</v>
+      </c>
+      <c r="C41" s="13"/>
+      <c r="E41" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F41" s="32">
+      <c r="F41" s="24">
         <v>0</v>
       </c>
       <c r="G41"/>
@@ -1985,14 +1938,13 @@
       <c r="I41"/>
     </row>
     <row r="42" ht="12" customHeight="1" spans="1:9">
-      <c r="A42" s="33"/>
-      <c r="B42" s="34" t="s">
+      <c r="A42" s="25"/>
+      <c r="B42" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="35"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="34" t="s">
+      <c r="C42" s="27"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="26" t="s">
         <v>22</v>
       </c>
       <c r="G42"/>
@@ -2000,11 +1952,11 @@
       <c r="I42"/>
     </row>
     <row r="43" ht="10" customHeight="1" spans="1:9">
-      <c r="A43" s="38"/>
-      <c r="B43" s="35"/>
-      <c r="C43" s="35"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="35"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="27"/>
       <c r="G43"/>
       <c r="H43"/>
       <c r="I43"/>
@@ -2021,48 +1973,45 @@
       <c r="I44"/>
     </row>
     <row r="45" ht="12" customHeight="1" spans="1:9">
-      <c r="A45" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" s="6"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F45" s="6"/>
+      <c r="A45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="6"/>
+      <c r="E45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F45" s="5"/>
       <c r="G45"/>
       <c r="H45"/>
       <c r="I45"/>
     </row>
     <row r="46" ht="12" customHeight="1" spans="1:9">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="10"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="9" t="s">
+      <c r="B46" s="9"/>
+      <c r="C46" s="10"/>
+      <c r="E46" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F46" s="10"/>
+      <c r="F46" s="9"/>
       <c r="G46"/>
       <c r="H46"/>
       <c r="I46"/>
     </row>
     <row r="47" ht="12" customHeight="1" spans="1:9">
-      <c r="A47" s="12" t="s">
+      <c r="A47" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C47" s="14"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="12" t="s">
+      <c r="C47" s="13"/>
+      <c r="E47" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F47" s="13" t="s">
+      <c r="F47" s="12" t="s">
         <v>4</v>
       </c>
       <c r="G47"/>
@@ -2070,18 +2019,17 @@
       <c r="I47"/>
     </row>
     <row r="48" ht="12" customHeight="1" spans="1:9">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="15" t="s">
+      <c r="C48" s="13"/>
+      <c r="E48" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="16" t="s">
+      <c r="F48" s="15" t="s">
         <v>6</v>
       </c>
       <c r="G48"/>
@@ -2089,18 +2037,17 @@
       <c r="I48"/>
     </row>
     <row r="49" customHeight="1" spans="1:9">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="17">
-        <v>0</v>
-      </c>
-      <c r="C49" s="18"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="17" t="s">
+      <c r="B49" s="16">
+        <v>0</v>
+      </c>
+      <c r="C49" s="17"/>
+      <c r="E49" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F49" s="17">
+      <c r="F49" s="16">
         <v>0</v>
       </c>
       <c r="G49"/>
@@ -2108,18 +2055,17 @@
       <c r="I49"/>
     </row>
     <row r="50" customHeight="1" spans="1:9">
-      <c r="A50" s="19" t="s">
+      <c r="A50" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B50" s="19">
-        <v>0</v>
-      </c>
-      <c r="C50" s="18"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="19" t="s">
+      <c r="B50" s="18">
+        <v>0</v>
+      </c>
+      <c r="C50" s="17"/>
+      <c r="E50" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F50" s="19">
+      <c r="F50" s="18">
         <v>0</v>
       </c>
       <c r="G50"/>
@@ -2127,18 +2073,17 @@
       <c r="I50"/>
     </row>
     <row r="51" customHeight="1" spans="1:9">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="19">
-        <v>0</v>
-      </c>
-      <c r="C51" s="18"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="19" t="s">
+      <c r="B51" s="18">
+        <v>0</v>
+      </c>
+      <c r="C51" s="17"/>
+      <c r="E51" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F51" s="19">
+      <c r="F51" s="18">
         <v>0</v>
       </c>
       <c r="G51"/>
@@ -2146,18 +2091,17 @@
       <c r="I51"/>
     </row>
     <row r="52" customHeight="1" spans="1:9">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B52" s="19">
-        <v>0</v>
-      </c>
-      <c r="C52" s="18"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="19" t="s">
+      <c r="B52" s="18">
+        <v>0</v>
+      </c>
+      <c r="C52" s="17"/>
+      <c r="E52" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F52" s="19">
+      <c r="F52" s="18">
         <v>0</v>
       </c>
       <c r="G52"/>
@@ -2165,18 +2109,17 @@
       <c r="I52"/>
     </row>
     <row r="53" customHeight="1" spans="1:9">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="19">
-        <v>0</v>
-      </c>
-      <c r="C53" s="18"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="19" t="s">
+      <c r="B53" s="18">
+        <v>0</v>
+      </c>
+      <c r="C53" s="17"/>
+      <c r="E53" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="19">
+      <c r="F53" s="18">
         <v>0</v>
       </c>
       <c r="G53"/>
@@ -2184,18 +2127,17 @@
       <c r="I53"/>
     </row>
     <row r="54" customHeight="1" spans="1:9">
-      <c r="A54" s="19" t="s">
+      <c r="A54" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B54" s="19">
-        <v>0</v>
-      </c>
-      <c r="C54" s="18"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="19" t="s">
+      <c r="B54" s="18">
+        <v>0</v>
+      </c>
+      <c r="C54" s="17"/>
+      <c r="E54" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F54" s="19">
+      <c r="F54" s="18">
         <v>0</v>
       </c>
       <c r="G54"/>
@@ -2203,18 +2145,17 @@
       <c r="I54"/>
     </row>
     <row r="55" customHeight="1" spans="1:9">
-      <c r="A55" s="19" t="s">
+      <c r="A55" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B55" s="19">
-        <v>0</v>
-      </c>
-      <c r="C55" s="18"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="19" t="s">
+      <c r="B55" s="18">
+        <v>0</v>
+      </c>
+      <c r="C55" s="17"/>
+      <c r="E55" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F55" s="19">
+      <c r="F55" s="18">
         <v>0</v>
       </c>
       <c r="G55"/>
@@ -2222,18 +2163,17 @@
       <c r="I55"/>
     </row>
     <row r="56" customHeight="1" spans="1:9">
-      <c r="A56" s="19" t="s">
+      <c r="A56" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B56" s="19">
-        <v>0</v>
-      </c>
-      <c r="C56" s="18"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="19" t="s">
+      <c r="B56" s="18">
+        <v>0</v>
+      </c>
+      <c r="C56" s="17"/>
+      <c r="E56" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F56" s="19">
+      <c r="F56" s="18">
         <v>0</v>
       </c>
       <c r="G56"/>
@@ -2241,18 +2181,17 @@
       <c r="I56"/>
     </row>
     <row r="57" customHeight="1" spans="1:9">
-      <c r="A57" s="20" t="s">
+      <c r="A57" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B57" s="20">
-        <v>0</v>
-      </c>
-      <c r="C57" s="18"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="20" t="s">
+      <c r="B57" s="19">
+        <v>0</v>
+      </c>
+      <c r="C57" s="17"/>
+      <c r="E57" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F57" s="20">
+      <c r="F57" s="19">
         <v>0</v>
       </c>
       <c r="G57"/>
@@ -2260,37 +2199,37 @@
       <c r="I57"/>
     </row>
     <row r="58" s="3" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A58" s="21" t="s">
+      <c r="A58" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B58" s="22">
-        <v>0</v>
-      </c>
-      <c r="C58" s="36"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="21" t="s">
+      <c r="B58" s="21">
+        <f>SUM(B49:B57)</f>
+        <v>0</v>
+      </c>
+      <c r="C58" s="28"/>
+      <c r="E58" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F58" s="22">
-        <v>0</v>
-      </c>
-      <c r="G58" s="37"/>
-      <c r="H58" s="37"/>
-      <c r="I58" s="37"/>
+      <c r="F58" s="21">
+        <f>SUM(F49:F57)</f>
+        <v>0</v>
+      </c>
+      <c r="G58" s="29"/>
+      <c r="H58" s="29"/>
+      <c r="I58" s="29"/>
     </row>
     <row r="59" customHeight="1" spans="1:9">
-      <c r="A59" s="17" t="s">
+      <c r="A59" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B59" s="24">
-        <v>0</v>
-      </c>
-      <c r="C59" s="25"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="17" t="s">
+      <c r="B59" s="16">
+        <v>0</v>
+      </c>
+      <c r="C59" s="17"/>
+      <c r="E59" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F59" s="24">
+      <c r="F59" s="16">
         <v>0</v>
       </c>
       <c r="G59"/>
@@ -2298,18 +2237,17 @@
       <c r="I59"/>
     </row>
     <row r="60" customHeight="1" spans="1:9">
-      <c r="A60" s="20" t="s">
+      <c r="A60" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B60" s="26">
-        <v>0</v>
-      </c>
-      <c r="C60" s="25"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="20" t="s">
+      <c r="B60" s="19">
+        <v>0</v>
+      </c>
+      <c r="C60" s="17"/>
+      <c r="E60" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F60" s="26">
+      <c r="F60" s="19">
         <v>0</v>
       </c>
       <c r="G60"/>
@@ -2317,18 +2255,17 @@
       <c r="I60"/>
     </row>
     <row r="61" customHeight="1" spans="1:9">
-      <c r="A61" s="27" t="s">
+      <c r="A61" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B61" s="28">
-        <v>0</v>
-      </c>
-      <c r="C61" s="23"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="29" t="s">
+      <c r="B61" s="22">
+        <v>0</v>
+      </c>
+      <c r="C61" s="13"/>
+      <c r="E61" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="F61" s="30">
+      <c r="F61" s="23">
         <v>0</v>
       </c>
       <c r="G61"/>
@@ -2336,18 +2273,17 @@
       <c r="I61"/>
     </row>
     <row r="62" customHeight="1" spans="1:9">
-      <c r="A62" s="27" t="s">
+      <c r="A62" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B62" s="28">
-        <v>0</v>
-      </c>
-      <c r="C62" s="23"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="27" t="s">
+      <c r="B62" s="22">
+        <v>0</v>
+      </c>
+      <c r="C62" s="13"/>
+      <c r="E62" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F62" s="28">
+      <c r="F62" s="22">
         <v>0</v>
       </c>
       <c r="G62"/>
@@ -2355,18 +2291,17 @@
       <c r="I62"/>
     </row>
     <row r="63" customHeight="1" spans="1:9">
-      <c r="A63" s="31" t="s">
+      <c r="A63" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B63" s="32">
-        <v>0</v>
-      </c>
-      <c r="C63" s="23"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="31" t="s">
+      <c r="B63" s="24">
+        <v>0</v>
+      </c>
+      <c r="C63" s="13"/>
+      <c r="E63" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F63" s="32">
+      <c r="F63" s="24">
         <v>0</v>
       </c>
       <c r="G63"/>
@@ -2374,14 +2309,13 @@
       <c r="I63"/>
     </row>
     <row r="64" ht="12" customHeight="1" spans="1:9">
-      <c r="A64" s="33"/>
-      <c r="B64" s="34" t="s">
+      <c r="A64" s="25"/>
+      <c r="B64" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C64" s="35"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="33"/>
-      <c r="F64" s="34" t="s">
+      <c r="C64" s="27"/>
+      <c r="E64" s="25"/>
+      <c r="F64" s="26" t="s">
         <v>22</v>
       </c>
       <c r="G64"/>

</xml_diff>